<commit_message>
added Week 2 training materials
</commit_message>
<xml_diff>
--- a/Setup and Installation/Required Software and Setup.xlsx
+++ b/Setup and Installation/Required Software and Setup.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Virtual Training\ACE\Sapient\PSI-2024 Nov ASDE BLR Batch 1\Setup and Installation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online Training\ACE\Sapient\PSI-2024 Nov ASDE BLR Batch 1\Setup and Installation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2B37FD-2D05-488B-8B87-B9EB379E938B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB983FB-FD10-4118-B325-E98B54266DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>Serial No.</t>
   </si>
@@ -127,18 +127,9 @@
     <t>https://www.jenkins.io/download/</t>
   </si>
   <si>
-    <t>https://podman-desktop.io/downloads/windows</t>
-  </si>
-  <si>
-    <t>https://developers.redhat.com/articles/2023/09/27/how-install-and-use-podman-desktop-windows#install_podman_desktop_on_windows</t>
-  </si>
-  <si>
     <t>SonarQube Server Version 10.7</t>
   </si>
   <si>
-    <t>** Install Podman as a container engine with guidance from Podman Desktop. Select options for Docker Compose and Kubectl CLI as well.</t>
-  </si>
-  <si>
     <t>https://dev.mysql.com/downloads/mysql/</t>
   </si>
   <si>
@@ -176,9 +167,6 @@
   </si>
   <si>
     <t>Node.js ver. 22.11.0(LTS)</t>
-  </si>
-  <si>
-    <t>Podman Desktop for Windows ver. 1.14.1</t>
   </si>
   <si>
     <t>Jenkins 2.479.1 LTS</t>
@@ -197,7 +185,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,12 +258,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF151515"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -300,7 +282,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -324,23 +306,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -622,11 +592,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -668,7 +638,7 @@
     <row r="4" spans="1:4">
       <c r="A4" s="2"/>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -679,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>3</v>
@@ -696,7 +666,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>4</v>
@@ -715,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>5</v>
@@ -735,13 +705,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -752,13 +722,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -769,7 +739,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>6</v>
@@ -786,7 +756,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>7</v>
@@ -800,7 +770,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>8</v>
@@ -836,8 +806,8 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="D24" s="19" t="s">
-        <v>50</v>
+      <c r="D24" s="15" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="21" customHeight="1">
@@ -845,7 +815,7 @@
         <v>11</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>11</v>
@@ -879,7 +849,7 @@
         <v>13</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>14</v>
@@ -891,96 +861,75 @@
     <row r="30" spans="1:4" ht="18.5">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:4" ht="43.5">
-      <c r="A31" s="18">
+    <row r="31" spans="1:4" ht="18.5">
+      <c r="A31" s="2">
         <v>14</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="17" t="s">
+      <c r="B31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="18.5">
+      <c r="A33" s="2">
+        <v>15</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="23">
-      <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="18.5">
-      <c r="A34" s="2">
-        <v>15</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="C33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18.5">
+      <c r="A35" s="2">
         <v>16</v>
       </c>
-      <c r="D34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="18.5">
-      <c r="A36" s="2">
-        <v>16</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="18.5">
-      <c r="A38" s="2">
-        <v>17</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="B35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="D39" s="14"/>
-    </row>
-    <row r="40" spans="1:4" ht="18.5">
-      <c r="A40" s="2"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="15"/>
-    </row>
-    <row r="42" spans="1:4" ht="18.5">
-      <c r="A42" s="2"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="44" spans="1:4" ht="18.5">
-      <c r="A44" s="2"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="5"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="2"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="2"/>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="2"/>
+      <c r="D35" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="D36" s="13"/>
+    </row>
+    <row r="37" spans="1:4" ht="18.5">
+      <c r="A37" s="2"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="14"/>
+    </row>
+    <row r="39" spans="1:4" ht="18.5">
+      <c r="A39" s="2"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+    </row>
+    <row r="41" spans="1:4" ht="18.5">
+      <c r="A41" s="2"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -994,7 +943,7 @@
     <hyperlink ref="C25" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="C23" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="C20" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C34" r:id="rId11" xr:uid="{0A06AE85-B4C8-459A-BA6F-EE69761E6BAD}"/>
+    <hyperlink ref="C31" r:id="rId11" xr:uid="{0A06AE85-B4C8-459A-BA6F-EE69761E6BAD}"/>
     <hyperlink ref="D6" r:id="rId12" xr:uid="{6A18C142-6FA8-4624-A662-412AD9FE64DB}"/>
     <hyperlink ref="D8" r:id="rId13" xr:uid="{EE1561DD-3E78-4247-AA20-FDD9457BDCF6}"/>
     <hyperlink ref="D10" r:id="rId14" xr:uid="{F23A5A18-F828-4EC3-9404-02E5C857E0EE}"/>
@@ -1006,14 +955,13 @@
     <hyperlink ref="D29" r:id="rId20" xr:uid="{87AD9AB9-194B-4737-AB65-6CD9BD1A2D78}"/>
     <hyperlink ref="C3" r:id="rId21" xr:uid="{1AEAFBBA-326F-476A-95A0-4717CA32DF5A}"/>
     <hyperlink ref="D3" r:id="rId22" xr:uid="{8A323149-832A-4791-B725-E82025A6B40F}"/>
-    <hyperlink ref="C36" r:id="rId23" xr:uid="{81DD06A2-8B33-4AC2-94E7-58FDB58EC193}"/>
-    <hyperlink ref="D36" r:id="rId24" xr:uid="{80ED40D2-6261-493D-B9D1-4C3E95861119}"/>
-    <hyperlink ref="C38" r:id="rId25" xr:uid="{9B507B12-1350-4589-B1D4-7EDD2F981557}"/>
-    <hyperlink ref="C31" r:id="rId26" xr:uid="{308EEECE-A66E-4746-BE27-C3B7EBEE1AFD}"/>
-    <hyperlink ref="C12" r:id="rId27" xr:uid="{90B5C688-835D-47CA-996A-6AB587DDCD00}"/>
-    <hyperlink ref="C14" r:id="rId28" xr:uid="{82B0F35B-DADD-4C33-8D23-39D16763531B}"/>
-    <hyperlink ref="D14" r:id="rId29" xr:uid="{3276829A-0F33-4456-A1C4-482DD6619727}"/>
-    <hyperlink ref="D12" r:id="rId30" xr:uid="{F3597BFD-B8CC-4D90-97B0-093B160D7C34}"/>
+    <hyperlink ref="C33" r:id="rId23" xr:uid="{81DD06A2-8B33-4AC2-94E7-58FDB58EC193}"/>
+    <hyperlink ref="D33" r:id="rId24" xr:uid="{80ED40D2-6261-493D-B9D1-4C3E95861119}"/>
+    <hyperlink ref="C35" r:id="rId25" xr:uid="{9B507B12-1350-4589-B1D4-7EDD2F981557}"/>
+    <hyperlink ref="C12" r:id="rId26" xr:uid="{90B5C688-835D-47CA-996A-6AB587DDCD00}"/>
+    <hyperlink ref="C14" r:id="rId27" xr:uid="{82B0F35B-DADD-4C33-8D23-39D16763531B}"/>
+    <hyperlink ref="D14" r:id="rId28" xr:uid="{3276829A-0F33-4456-A1C4-482DD6619727}"/>
+    <hyperlink ref="D12" r:id="rId29" xr:uid="{F3597BFD-B8CC-4D90-97B0-093B160D7C34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>